<commit_message>
Cambio en nombre de recurso
Cambio en nombre de recurso
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion14/escaleta_CN_11_14.xlsx
+++ b/fuentes/contenidos/grado11/guion14/escaleta_CN_11_14.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado11\guion14\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -408,16 +413,10 @@
     <t>La ruptura heterolítica</t>
   </si>
   <si>
-    <t>Los tipos de reactivos</t>
-  </si>
-  <si>
     <t>Nucleófilos</t>
   </si>
   <si>
     <t>Electrófilos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secuencia de imágenes que permite exponer las clases de ruptura de enlaces covalente y los reactivos electrófilos y nucleófilos </t>
   </si>
   <si>
     <t>RM</t>
@@ -559,12 +558,6 @@
     <t>Recurso F13B-01</t>
   </si>
   <si>
-    <t>Completa la reacción con el reactivo o producto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad que permite identificar los reactivos o productos en reacciones químicas que incluyen hidrocarburos </t>
-  </si>
-  <si>
     <t>Recurso M7A-02</t>
   </si>
   <si>
@@ -700,12 +693,6 @@
     <t>Recurso M5A-03</t>
   </si>
   <si>
-    <t>La ruptura de enlaces y las clases de reactivos</t>
-  </si>
-  <si>
-    <t>Reconoce los mecanismos de ruptura y el tipo de reactivo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Actividad para identificar las ruptura de enlace y las especies nucleófilas y electrófilas </t>
   </si>
   <si>
@@ -772,9 +759,6 @@
     <t>Recurso F7-02</t>
   </si>
   <si>
-    <t>Escribe el nombre del reactivo o del producto</t>
-  </si>
-  <si>
     <t>Actividad que permite identificar las sustancias que intervienen en la obtención y las propiedades químicas de los alcoholes</t>
   </si>
   <si>
@@ -784,9 +768,6 @@
     <t>Identifica la sustancia que interviene en la reacción</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad que permite reconocer los reactivos o productos en reacciones que incluyen aldehídos </t>
-  </si>
-  <si>
     <t>Recurso M6A-02</t>
   </si>
   <si>
@@ -802,9 +783,6 @@
     <t>Reconoce la sustancia que interviene en la reacción</t>
   </si>
   <si>
-    <t>Actividad  para identificar reactivos o productos en las reacciones de síntesis y propiedades químicas de las cetonas</t>
-  </si>
-  <si>
     <t>Recurso M5A-01</t>
   </si>
   <si>
@@ -850,9 +828,6 @@
     <t xml:space="preserve">Identifica las sustancias que intervienen en las reacciones de los ésteres </t>
   </si>
   <si>
-    <t>Actividad para reconocer los reactivos y productos de reacciones que involucran ésteres</t>
-  </si>
-  <si>
     <t>Recurso M9B-01</t>
   </si>
   <si>
@@ -953,6 +928,36 @@
   </si>
   <si>
     <t>RF_01_02_CO</t>
+  </si>
+  <si>
+    <t>Los tipos de reactantes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad que permite identificar los reactantes o productos en reacciones químicas que incluyen hidrocarburos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad que permite reconocer los reactantes o productos en reacciones que incluyen aldehídos </t>
+  </si>
+  <si>
+    <t>Actividad  para identificar reactantes o productos en las reacciones de síntesis y propiedades químicas de las cetonas</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer los reactantes y productos de reacciones que involucran ésteres</t>
+  </si>
+  <si>
+    <t>La ruptura de enlaces y las clases de reactantes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secuencia de imágenes que permite exponer las clases de ruptura de enlaces covalente y los reactantes electrófilos y nucleófilos </t>
+  </si>
+  <si>
+    <t>Reconoce los mecanismos de ruptura y el tipo de reactantes</t>
+  </si>
+  <si>
+    <t>Completa la reacción con el reactante o producto</t>
+  </si>
+  <si>
+    <t>Escribe el nombre del reactante o del producto</t>
   </si>
 </sst>
 </file>
@@ -1164,16 +1169,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1213,24 +1236,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1309,7 +1314,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1344,7 +1349,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1555,9 +1560,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q71" sqref="Q71:U71"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,94 +1590,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="18" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="M1" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="25" t="s">
+      <c r="N1" s="43"/>
+      <c r="O1" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="Q1" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="44" t="s">
+      <c r="R1" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="40" t="s">
+      <c r="S1" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="42" t="s">
+      <c r="T1" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="40" t="s">
+      <c r="U1" s="25" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="18" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="32"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="38"/>
       <c r="M2" s="19" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="41"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="26"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1692,7 +1697,7 @@
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="16" t="s">
-        <v>223</v>
+        <v>303</v>
       </c>
       <c r="H3" s="20">
         <v>1</v>
@@ -1701,7 +1706,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>131</v>
+        <v>304</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1721,16 +1726,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="T3" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="U3" s="10" t="s">
         <v>133</v>
-      </c>
-      <c r="T3" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1817,10 +1822,10 @@
         <v>124</v>
       </c>
       <c r="E6" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="20"/>
@@ -1852,13 +1857,13 @@
         <v>124</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>128</v>
+        <v>298</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>224</v>
+        <v>305</v>
       </c>
       <c r="H7" s="20">
         <v>2</v>
@@ -1867,7 +1872,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -1887,16 +1892,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S7" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="U7" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T7" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="U7" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1913,11 +1918,11 @@
         <v>124</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H8" s="20">
         <v>3</v>
@@ -1926,7 +1931,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -1936,7 +1941,7 @@
       </c>
       <c r="M8" s="8"/>
       <c r="N8" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O8" s="9"/>
       <c r="P8" s="9" t="s">
@@ -1946,16 +1951,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S8" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="U8" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T8" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="U8" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1969,12 +1974,12 @@
         <v>123</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="9"/>
       <c r="G9" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H9" s="20">
         <v>4</v>
@@ -1983,7 +1988,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>20</v>
@@ -2003,16 +2008,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="T9" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="S9" s="10" t="s">
+      <c r="U9" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="T9" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="U9" s="10" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2026,10 +2031,10 @@
         <v>123</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="16"/>
@@ -2059,10 +2064,10 @@
         <v>123</v>
       </c>
       <c r="D11" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>143</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>145</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="16"/>
@@ -2092,10 +2097,10 @@
         <v>123</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="16"/>
@@ -2125,14 +2130,14 @@
         <v>123</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="H13" s="20">
         <v>5</v>
@@ -2141,7 +2146,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
@@ -2161,16 +2166,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S13" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T13" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="U13" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T13" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="U13" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2184,14 +2189,14 @@
         <v>123</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H14" s="20">
         <v>6</v>
@@ -2200,7 +2205,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>20</v>
@@ -2210,7 +2215,7 @@
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="9" t="s">
@@ -2220,16 +2225,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S14" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T14" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="U14" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T14" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="U14" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2243,12 +2248,12 @@
         <v>123</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="H15" s="20">
         <v>7</v>
@@ -2257,7 +2262,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2277,16 +2282,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S15" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="T15" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="U15" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="T15" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="U15" s="10" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2300,13 +2305,13 @@
         <v>123</v>
       </c>
       <c r="D16" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>158</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="9"/>
@@ -2335,13 +2340,13 @@
         <v>123</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E17" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>159</v>
       </c>
       <c r="G17" s="16"/>
       <c r="H17" s="9"/>
@@ -2370,13 +2375,13 @@
         <v>123</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="9"/>
@@ -2405,16 +2410,16 @@
         <v>123</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="H19" s="20">
         <v>8</v>
@@ -2423,7 +2428,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2443,16 +2448,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S19" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T19" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="U19" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T19" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="U19" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2466,13 +2471,13 @@
         <v>123</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="9"/>
@@ -2501,13 +2506,13 @@
         <v>123</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E21" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="9"/>
@@ -2536,13 +2541,13 @@
         <v>123</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="9"/>
@@ -2571,16 +2576,16 @@
         <v>123</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H23" s="20">
         <v>9</v>
@@ -2589,7 +2594,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2609,16 +2614,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S23" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T23" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="U23" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T23" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="U23" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2632,13 +2637,13 @@
         <v>123</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="9"/>
@@ -2667,13 +2672,13 @@
         <v>123</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E25" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>169</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="9"/>
@@ -2702,13 +2707,13 @@
         <v>123</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="9"/>
@@ -2737,16 +2742,16 @@
         <v>123</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="H27" s="20">
         <v>10</v>
@@ -2755,7 +2760,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>20</v>
@@ -2775,16 +2780,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S27" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T27" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="U27" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T27" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="U27" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2798,13 +2803,13 @@
         <v>123</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="20"/>
@@ -2833,13 +2838,13 @@
         <v>123</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="20"/>
@@ -2868,13 +2873,13 @@
         <v>123</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E30" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>172</v>
       </c>
       <c r="G30" s="16"/>
       <c r="H30" s="20"/>
@@ -2903,16 +2908,16 @@
         <v>123</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H31" s="20">
         <v>11</v>
@@ -2921,7 +2926,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>20</v>
@@ -2941,16 +2946,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S31" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="T31" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="U31" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="T31" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="U31" s="10" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2964,16 +2969,16 @@
         <v>123</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>176</v>
+        <v>306</v>
       </c>
       <c r="H32" s="20">
         <v>12</v>
@@ -2982,7 +2987,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>177</v>
+        <v>299</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>20</v>
@@ -3002,16 +3007,16 @@
         <v>6</v>
       </c>
       <c r="R32" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S32" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T32" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="U32" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T32" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="U32" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3025,14 +3030,14 @@
         <v>123</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H33" s="20">
         <v>13</v>
@@ -3041,7 +3046,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>20</v>
@@ -3051,7 +3056,7 @@
       </c>
       <c r="M33" s="8"/>
       <c r="N33" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O33" s="9"/>
       <c r="P33" s="9" t="s">
@@ -3061,16 +3066,16 @@
         <v>6</v>
       </c>
       <c r="R33" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S33" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T33" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="U33" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T33" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="U33" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3084,14 +3089,14 @@
         <v>123</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="16" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="H34" s="20">
         <v>14</v>
@@ -3100,7 +3105,7 @@
         <v>19</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
@@ -3120,16 +3125,16 @@
         <v>6</v>
       </c>
       <c r="R34" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S34" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="T34" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="U34" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="T34" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="U34" s="10" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3143,13 +3148,13 @@
         <v>123</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G35" s="16"/>
       <c r="H35" s="9"/>
@@ -3178,13 +3183,13 @@
         <v>123</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G36" s="16"/>
       <c r="H36" s="9"/>
@@ -3213,16 +3218,16 @@
         <v>123</v>
       </c>
       <c r="D37" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="F37" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E37" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>185</v>
-      </c>
       <c r="G37" s="16" t="s">
-        <v>247</v>
+        <v>307</v>
       </c>
       <c r="H37" s="20">
         <v>15</v>
@@ -3231,7 +3236,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>20</v>
@@ -3251,16 +3256,16 @@
         <v>6</v>
       </c>
       <c r="R37" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S37" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T37" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="U37" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T37" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="U37" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3274,13 +3279,13 @@
         <v>123</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G38" s="16"/>
       <c r="H38" s="9"/>
@@ -3309,13 +3314,13 @@
         <v>123</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G39" s="16"/>
       <c r="H39" s="9"/>
@@ -3344,13 +3349,13 @@
         <v>123</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="9"/>
@@ -3379,13 +3384,13 @@
         <v>123</v>
       </c>
       <c r="D41" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="F41" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>185</v>
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="9"/>
@@ -3414,16 +3419,16 @@
         <v>123</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="H42" s="20">
         <v>16</v>
@@ -3432,7 +3437,7 @@
         <v>20</v>
       </c>
       <c r="J42" s="17" t="s">
-        <v>251</v>
+        <v>300</v>
       </c>
       <c r="K42" s="7" t="s">
         <v>20</v>
@@ -3452,16 +3457,16 @@
         <v>6</v>
       </c>
       <c r="R42" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S42" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T42" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="U42" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T42" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="U42" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3475,13 +3480,13 @@
         <v>123</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G43" s="16"/>
       <c r="H43" s="9"/>
@@ -3510,13 +3515,13 @@
         <v>123</v>
       </c>
       <c r="D44" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F44" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>185</v>
       </c>
       <c r="G44" s="16"/>
       <c r="H44" s="9"/>
@@ -3545,16 +3550,16 @@
         <v>123</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="H45" s="20">
         <v>17</v>
@@ -3563,7 +3568,7 @@
         <v>19</v>
       </c>
       <c r="J45" s="17" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="K45" s="7" t="s">
         <v>20</v>
@@ -3583,16 +3588,16 @@
         <v>6</v>
       </c>
       <c r="R45" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S45" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="T45" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="U45" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="T45" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="U45" s="10" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3606,16 +3611,16 @@
         <v>123</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="H46" s="20">
         <v>18</v>
@@ -3624,7 +3629,7 @@
         <v>20</v>
       </c>
       <c r="J46" s="17" t="s">
-        <v>257</v>
+        <v>301</v>
       </c>
       <c r="K46" s="7" t="s">
         <v>20</v>
@@ -3644,16 +3649,16 @@
         <v>6</v>
       </c>
       <c r="R46" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S46" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T46" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="U46" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T46" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="U46" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3667,13 +3672,13 @@
         <v>123</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="9"/>
@@ -3702,16 +3707,16 @@
         <v>123</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="H48" s="20">
         <v>19</v>
@@ -3720,7 +3725,7 @@
         <v>20</v>
       </c>
       <c r="J48" s="17" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="K48" s="7" t="s">
         <v>20</v>
@@ -3740,16 +3745,16 @@
         <v>6</v>
       </c>
       <c r="R48" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S48" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T48" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="U48" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T48" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="U48" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3763,16 +3768,16 @@
         <v>123</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="H49" s="20">
         <v>20</v>
@@ -3781,7 +3786,7 @@
         <v>20</v>
       </c>
       <c r="J49" s="17" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="K49" s="7" t="s">
         <v>20</v>
@@ -3801,16 +3806,16 @@
         <v>6</v>
       </c>
       <c r="R49" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S49" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T49" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="U49" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T49" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="U49" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3824,14 +3829,14 @@
         <v>123</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F50" s="9"/>
       <c r="G50" s="16" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="H50" s="20">
         <v>21</v>
@@ -3840,7 +3845,7 @@
         <v>20</v>
       </c>
       <c r="J50" s="17" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="K50" s="7" t="s">
         <v>20</v>
@@ -3850,7 +3855,7 @@
       </c>
       <c r="M50" s="8"/>
       <c r="N50" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O50" s="9"/>
       <c r="P50" s="9" t="s">
@@ -3860,16 +3865,16 @@
         <v>6</v>
       </c>
       <c r="R50" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S50" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T50" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="U50" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T50" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="U50" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3883,14 +3888,14 @@
         <v>123</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="16" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="H51" s="20">
         <v>22</v>
@@ -3899,7 +3904,7 @@
         <v>19</v>
       </c>
       <c r="J51" s="17" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="K51" s="7" t="s">
         <v>20</v>
@@ -3919,16 +3924,16 @@
         <v>6</v>
       </c>
       <c r="R51" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S51" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="T51" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="U51" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="T51" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="U51" s="10" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3942,13 +3947,13 @@
         <v>123</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G52" s="16"/>
       <c r="H52" s="9"/>
@@ -3977,13 +3982,13 @@
         <v>123</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G53" s="16"/>
       <c r="H53" s="9"/>
@@ -4012,16 +4017,16 @@
         <v>123</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="H54" s="20">
         <v>23</v>
@@ -4030,7 +4035,7 @@
         <v>20</v>
       </c>
       <c r="J54" s="17" t="s">
-        <v>273</v>
+        <v>302</v>
       </c>
       <c r="K54" s="7" t="s">
         <v>20</v>
@@ -4050,16 +4055,16 @@
         <v>6</v>
       </c>
       <c r="R54" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S54" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T54" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="U54" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T54" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="U54" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4073,16 +4078,16 @@
         <v>123</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="H55" s="20">
         <v>24</v>
@@ -4091,7 +4096,7 @@
         <v>20</v>
       </c>
       <c r="J55" s="17" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="K55" s="7" t="s">
         <v>20</v>
@@ -4104,7 +4109,7 @@
         <v>34</v>
       </c>
       <c r="O55" s="22" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="P55" s="9" t="s">
         <v>20</v>
@@ -4113,16 +4118,16 @@
         <v>6</v>
       </c>
       <c r="R55" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S55" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T55" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="U55" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T55" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="U55" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4136,13 +4141,13 @@
         <v>123</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G56" s="16"/>
       <c r="H56" s="9"/>
@@ -4171,13 +4176,13 @@
         <v>123</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G57" s="16"/>
       <c r="H57" s="9"/>
@@ -4206,13 +4211,13 @@
         <v>123</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G58" s="16"/>
       <c r="H58" s="9"/>
@@ -4241,13 +4246,13 @@
         <v>123</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G59" s="16"/>
       <c r="H59" s="9"/>
@@ -4276,13 +4281,13 @@
         <v>123</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G60" s="16"/>
       <c r="H60" s="9"/>
@@ -4311,16 +4316,16 @@
         <v>123</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G61" s="16" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="H61" s="20">
         <v>25</v>
@@ -4329,7 +4334,7 @@
         <v>20</v>
       </c>
       <c r="J61" s="17" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="K61" s="7" t="s">
         <v>20</v>
@@ -4349,16 +4354,16 @@
         <v>6</v>
       </c>
       <c r="R61" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S61" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T61" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="U61" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T61" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="U61" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4372,13 +4377,13 @@
         <v>123</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G62" s="16"/>
       <c r="H62" s="9"/>
@@ -4407,16 +4412,16 @@
         <v>123</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G63" s="16" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="H63" s="20">
         <v>26</v>
@@ -4425,7 +4430,7 @@
         <v>20</v>
       </c>
       <c r="J63" s="17" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="K63" s="7" t="s">
         <v>20</v>
@@ -4445,16 +4450,16 @@
         <v>6</v>
       </c>
       <c r="R63" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S63" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T63" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U63" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T63" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="U63" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4468,16 +4473,16 @@
         <v>123</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G64" s="16" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="H64" s="20">
         <v>27</v>
@@ -4486,7 +4491,7 @@
         <v>20</v>
       </c>
       <c r="J64" s="17" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="K64" s="7" t="s">
         <v>20</v>
@@ -4506,16 +4511,16 @@
         <v>6</v>
       </c>
       <c r="R64" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S64" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T64" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="U64" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T64" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="U64" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4529,14 +4534,14 @@
         <v>123</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="16" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="H65" s="20">
         <v>28</v>
@@ -4545,7 +4550,7 @@
         <v>20</v>
       </c>
       <c r="J65" s="17" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="K65" s="7" t="s">
         <v>20</v>
@@ -4555,7 +4560,7 @@
       </c>
       <c r="M65" s="8"/>
       <c r="N65" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O65" s="9"/>
       <c r="P65" s="9" t="s">
@@ -4565,16 +4570,16 @@
         <v>6</v>
       </c>
       <c r="R65" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S65" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T65" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="U65" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T65" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="U65" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4588,14 +4593,14 @@
         <v>123</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="16" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="H66" s="20">
         <v>29</v>
@@ -4604,7 +4609,7 @@
         <v>19</v>
       </c>
       <c r="J66" s="17" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="K66" s="7" t="s">
         <v>20</v>
@@ -4624,16 +4629,16 @@
         <v>6</v>
       </c>
       <c r="R66" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S66" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="T66" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="U66" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="T66" s="12" t="s">
-        <v>295</v>
-      </c>
-      <c r="U66" s="10" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4647,13 +4652,13 @@
         <v>123</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G67" s="16"/>
       <c r="H67" s="9"/>
@@ -4682,13 +4687,13 @@
         <v>123</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G68" s="16"/>
       <c r="H68" s="9"/>
@@ -4717,13 +4722,13 @@
         <v>123</v>
       </c>
       <c r="D69" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E69" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E69" s="13" t="s">
-        <v>211</v>
-      </c>
       <c r="F69" s="9" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G69" s="16"/>
       <c r="H69" s="9"/>
@@ -4752,16 +4757,16 @@
         <v>123</v>
       </c>
       <c r="D70" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E70" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E70" s="13" t="s">
-        <v>211</v>
-      </c>
       <c r="F70" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="H70" s="20">
         <v>30</v>
@@ -4770,7 +4775,7 @@
         <v>20</v>
       </c>
       <c r="J70" s="17" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="K70" s="7" t="s">
         <v>20</v>
@@ -4790,16 +4795,16 @@
         <v>6</v>
       </c>
       <c r="R70" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S70" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T70" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="U70" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T70" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="U70" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4813,14 +4818,14 @@
         <v>123</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E71" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F71" s="9"/>
       <c r="G71" s="16" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="H71" s="20">
         <v>31</v>
@@ -4829,7 +4834,7 @@
         <v>20</v>
       </c>
       <c r="J71" s="17" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="K71" s="7" t="s">
         <v>20</v>
@@ -4839,7 +4844,7 @@
       </c>
       <c r="M71" s="8"/>
       <c r="N71" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O71" s="9"/>
       <c r="P71" s="9" t="s">
@@ -4849,16 +4854,16 @@
         <v>6</v>
       </c>
       <c r="R71" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S71" s="10" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="T71" s="12" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="U71" s="10" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
     </row>
     <row r="72" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4872,12 +4877,12 @@
         <v>123</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E72" s="13"/>
       <c r="F72" s="9"/>
       <c r="G72" s="16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H72" s="20">
         <v>32</v>
@@ -4886,7 +4891,7 @@
         <v>20</v>
       </c>
       <c r="J72" s="17" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="K72" s="7" t="s">
         <v>20</v>
@@ -4906,16 +4911,16 @@
         <v>6</v>
       </c>
       <c r="R72" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S72" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T72" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="U72" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T72" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="U72" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4929,12 +4934,12 @@
         <v>123</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E73" s="13"/>
       <c r="F73" s="9"/>
       <c r="G73" s="16" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="H73" s="20">
         <v>33</v>
@@ -4943,7 +4948,7 @@
         <v>20</v>
       </c>
       <c r="J73" s="17" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="K73" s="7" t="s">
         <v>20</v>
@@ -4963,16 +4968,16 @@
         <v>6</v>
       </c>
       <c r="R73" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S73" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T73" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="U73" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T73" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="U73" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4986,7 +4991,7 @@
         <v>123</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E74" s="13"/>
       <c r="F74" s="9"/>
@@ -5000,7 +5005,7 @@
         <v>20</v>
       </c>
       <c r="J74" s="17" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K74" s="7" t="s">
         <v>20</v>
@@ -5031,12 +5036,12 @@
         <v>123</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E75" s="13"/>
       <c r="F75" s="9"/>
       <c r="G75" s="16" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H75" s="20">
         <v>35</v>
@@ -5045,7 +5050,7 @@
         <v>20</v>
       </c>
       <c r="J75" s="17" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="K75" s="7" t="s">
         <v>20</v>
@@ -5065,16 +5070,16 @@
         <v>6</v>
       </c>
       <c r="R75" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S75" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T75" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="U75" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T75" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="U75" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -5091,7 +5096,7 @@
       <c r="E76" s="13"/>
       <c r="F76" s="9"/>
       <c r="G76" s="16" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="H76" s="20">
         <v>36</v>
@@ -5100,7 +5105,7 @@
         <v>20</v>
       </c>
       <c r="J76" s="17" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="K76" s="7" t="s">
         <v>20</v>
@@ -5120,16 +5125,16 @@
         <v>6</v>
       </c>
       <c r="R76" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S76" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="T76" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="U76" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="T76" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="U76" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
@@ -5495,12 +5500,6 @@
     <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5515,6 +5514,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O55" r:id="rId1"/>

</xml_diff>

<commit_message>
Eliminar un recurso F
Eliminar un recurso F
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion14/escaleta_CN_11_14.xlsx
+++ b/fuentes/contenidos/grado11/guion14/escaleta_CN_11_14.xlsx
@@ -1186,16 +1186,55 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1237,45 +1276,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1604,8 +1604,8 @@
   <dimension ref="A1:U289"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H2"/>
+      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,94 +1633,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="18" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="36"/>
-      <c r="O1" s="24" t="s">
+      <c r="N1" s="53"/>
+      <c r="O1" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="43" t="s">
+      <c r="R1" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="41" t="s">
+      <c r="T1" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="35" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="18" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="31"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="48"/>
       <c r="M2" s="19" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="40"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="36"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -2442,64 +2442,64 @@
       <c r="T18" s="12"/>
       <c r="U18" s="10"/>
     </row>
-    <row r="19" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+    <row r="19" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="G19" s="46" t="s">
+      <c r="G19" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="H19" s="47">
+      <c r="H19" s="24">
         <v>8</v>
       </c>
-      <c r="I19" s="45" t="s">
+      <c r="I19" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="46" t="s">
+      <c r="J19" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="K19" s="45" t="s">
+      <c r="K19" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="45" t="s">
+      <c r="L19" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45" t="s">
+      <c r="M19" s="22"/>
+      <c r="N19" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46" t="s">
+      <c r="O19" s="23"/>
+      <c r="P19" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="46">
+      <c r="Q19" s="23">
         <v>6</v>
       </c>
-      <c r="R19" s="46" t="s">
+      <c r="R19" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="S19" s="46" t="s">
+      <c r="S19" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="T19" s="46" t="s">
+      <c r="T19" s="23" t="s">
         <v>231</v>
       </c>
-      <c r="U19" s="46" t="s">
+      <c r="U19" s="23" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2608,64 +2608,64 @@
       <c r="T22" s="12"/>
       <c r="U22" s="10"/>
     </row>
-    <row r="23" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
+    <row r="23" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="E23" s="46" t="s">
+      <c r="E23" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="F23" s="46" t="s">
+      <c r="F23" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="G23" s="46" t="s">
+      <c r="G23" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="H23" s="47">
+      <c r="H23" s="24">
         <v>9</v>
       </c>
-      <c r="I23" s="45" t="s">
+      <c r="I23" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="46" t="s">
+      <c r="J23" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="K23" s="45" t="s">
+      <c r="K23" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="45" t="s">
+      <c r="L23" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45" t="s">
+      <c r="M23" s="22"/>
+      <c r="N23" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46" t="s">
+      <c r="O23" s="23"/>
+      <c r="P23" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="46">
+      <c r="Q23" s="23">
         <v>6</v>
       </c>
-      <c r="R23" s="46" t="s">
+      <c r="R23" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="S23" s="46" t="s">
+      <c r="S23" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="T23" s="46" t="s">
+      <c r="T23" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="U23" s="46" t="s">
+      <c r="U23" s="23" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2774,64 +2774,64 @@
       <c r="T26" s="12"/>
       <c r="U26" s="10"/>
     </row>
-    <row r="27" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="45" t="s">
+    <row r="27" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="C27" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="E27" s="46" t="s">
+      <c r="E27" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="F27" s="46" t="s">
+      <c r="F27" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="G27" s="46" t="s">
+      <c r="G27" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="H27" s="47">
+      <c r="H27" s="24">
         <v>10</v>
       </c>
-      <c r="I27" s="45" t="s">
+      <c r="I27" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="46" t="s">
+      <c r="J27" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="K27" s="45" t="s">
+      <c r="K27" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L27" s="45" t="s">
+      <c r="L27" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="45"/>
-      <c r="N27" s="45" t="s">
+      <c r="M27" s="22"/>
+      <c r="N27" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="O27" s="46"/>
-      <c r="P27" s="46" t="s">
+      <c r="O27" s="23"/>
+      <c r="P27" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="46">
+      <c r="Q27" s="23">
         <v>6</v>
       </c>
-      <c r="R27" s="46" t="s">
+      <c r="R27" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="S27" s="46" t="s">
+      <c r="S27" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="T27" s="46" t="s">
+      <c r="T27" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="U27" s="46" t="s">
+      <c r="U27" s="23" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3001,64 +3001,64 @@
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:21" s="55" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="50" t="s">
+    <row r="32" spans="1:21" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="53" t="s">
+      <c r="B32" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="53" t="s">
+      <c r="C32" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D32" s="53" t="s">
+      <c r="D32" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="F32" s="53" t="s">
+      <c r="F32" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="G32" s="53" t="s">
+      <c r="G32" s="30" t="s">
         <v>306</v>
       </c>
-      <c r="H32" s="54">
+      <c r="H32" s="31">
         <v>12</v>
       </c>
-      <c r="I32" s="50" t="s">
+      <c r="I32" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J32" s="53" t="s">
+      <c r="J32" s="30" t="s">
         <v>299</v>
       </c>
-      <c r="K32" s="50" t="s">
+      <c r="K32" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="L32" s="50" t="s">
+      <c r="L32" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="50"/>
-      <c r="N32" s="50" t="s">
+      <c r="M32" s="27"/>
+      <c r="N32" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="O32" s="53"/>
-      <c r="P32" s="53" t="s">
+      <c r="O32" s="30"/>
+      <c r="P32" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="53">
+      <c r="Q32" s="30">
         <v>6</v>
       </c>
-      <c r="R32" s="53" t="s">
+      <c r="R32" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="S32" s="53" t="s">
+      <c r="S32" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="T32" s="53" t="s">
+      <c r="T32" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="U32" s="53" t="s">
+      <c r="U32" s="30" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3250,64 +3250,64 @@
       <c r="T36" s="12"/>
       <c r="U36" s="10"/>
     </row>
-    <row r="37" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="45" t="s">
+    <row r="37" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C37" s="46" t="s">
+      <c r="C37" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D37" s="46" t="s">
+      <c r="D37" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="E37" s="46" t="s">
+      <c r="E37" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="F37" s="46" t="s">
+      <c r="F37" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="G37" s="46" t="s">
+      <c r="G37" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="H37" s="47">
+      <c r="H37" s="24">
         <v>15</v>
       </c>
-      <c r="I37" s="45" t="s">
+      <c r="I37" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J37" s="46" t="s">
+      <c r="J37" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="K37" s="45" t="s">
+      <c r="K37" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L37" s="45" t="s">
+      <c r="L37" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45" t="s">
+      <c r="M37" s="22"/>
+      <c r="N37" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="O37" s="46"/>
-      <c r="P37" s="46" t="s">
+      <c r="O37" s="23"/>
+      <c r="P37" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q37" s="46">
+      <c r="Q37" s="23">
         <v>6</v>
       </c>
-      <c r="R37" s="46" t="s">
+      <c r="R37" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="S37" s="46" t="s">
+      <c r="S37" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="T37" s="46" t="s">
+      <c r="T37" s="23" t="s">
         <v>242</v>
       </c>
-      <c r="U37" s="46" t="s">
+      <c r="U37" s="23" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3451,64 +3451,64 @@
       <c r="T41" s="12"/>
       <c r="U41" s="10"/>
     </row>
-    <row r="42" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="45" t="s">
+    <row r="42" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="46" t="s">
+      <c r="C42" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D42" s="46" t="s">
+      <c r="D42" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="E42" s="46" t="s">
+      <c r="E42" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="F42" s="46" t="s">
+      <c r="F42" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="G42" s="46" t="s">
+      <c r="G42" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="H42" s="47">
+      <c r="H42" s="24">
         <v>16</v>
       </c>
-      <c r="I42" s="45" t="s">
+      <c r="I42" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J42" s="46" t="s">
+      <c r="J42" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="K42" s="45" t="s">
+      <c r="K42" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L42" s="45" t="s">
+      <c r="L42" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45" t="s">
+      <c r="M42" s="22"/>
+      <c r="N42" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="O42" s="46"/>
-      <c r="P42" s="46" t="s">
+      <c r="O42" s="23"/>
+      <c r="P42" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q42" s="46">
+      <c r="Q42" s="23">
         <v>6</v>
       </c>
-      <c r="R42" s="46" t="s">
+      <c r="R42" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="S42" s="46" t="s">
+      <c r="S42" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="T42" s="46" t="s">
+      <c r="T42" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="U42" s="46" t="s">
+      <c r="U42" s="23" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3582,125 +3582,125 @@
       <c r="T44" s="12"/>
       <c r="U44" s="10"/>
     </row>
-    <row r="45" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="45" t="s">
+    <row r="45" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C45" s="46" t="s">
+      <c r="C45" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D45" s="46" t="s">
+      <c r="D45" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="E45" s="46" t="s">
+      <c r="E45" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="F45" s="46" t="s">
+      <c r="F45" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="G45" s="46" t="s">
+      <c r="G45" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="H45" s="47">
+      <c r="H45" s="24">
         <v>17</v>
       </c>
-      <c r="I45" s="45" t="s">
+      <c r="I45" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="J45" s="46" t="s">
+      <c r="J45" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="K45" s="45" t="s">
+      <c r="K45" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L45" s="45" t="s">
+      <c r="L45" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M45" s="45" t="s">
+      <c r="M45" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="N45" s="45"/>
-      <c r="O45" s="46"/>
-      <c r="P45" s="46" t="s">
+      <c r="N45" s="22"/>
+      <c r="O45" s="23"/>
+      <c r="P45" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q45" s="46">
+      <c r="Q45" s="23">
         <v>6</v>
       </c>
-      <c r="R45" s="46" t="s">
+      <c r="R45" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="S45" s="46" t="s">
+      <c r="S45" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="T45" s="46" t="s">
+      <c r="T45" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="U45" s="46" t="s">
+      <c r="U45" s="23" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="45" t="s">
+    <row r="46" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C46" s="46" t="s">
+      <c r="C46" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D46" s="46" t="s">
+      <c r="D46" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="E46" s="46" t="s">
+      <c r="E46" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="F46" s="46" t="s">
+      <c r="F46" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="G46" s="46" t="s">
+      <c r="G46" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="H46" s="47">
+      <c r="H46" s="24">
         <v>18</v>
       </c>
-      <c r="I46" s="45" t="s">
+      <c r="I46" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J46" s="46" t="s">
+      <c r="J46" s="23" t="s">
         <v>301</v>
       </c>
-      <c r="K46" s="45" t="s">
+      <c r="K46" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L46" s="45" t="s">
+      <c r="L46" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M46" s="45"/>
-      <c r="N46" s="45" t="s">
+      <c r="M46" s="22"/>
+      <c r="N46" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="O46" s="46"/>
-      <c r="P46" s="46" t="s">
+      <c r="O46" s="23"/>
+      <c r="P46" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q46" s="46">
+      <c r="Q46" s="23">
         <v>6</v>
       </c>
-      <c r="R46" s="46" t="s">
+      <c r="R46" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="S46" s="46" t="s">
+      <c r="S46" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="T46" s="46" t="s">
+      <c r="T46" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="U46" s="46" t="s">
+      <c r="U46" s="23" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3739,125 +3739,125 @@
       <c r="T47" s="12"/>
       <c r="U47" s="10"/>
     </row>
-    <row r="48" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="45" t="s">
+    <row r="48" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B48" s="46" t="s">
+      <c r="B48" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C48" s="46" t="s">
+      <c r="C48" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D48" s="46" t="s">
+      <c r="D48" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="E48" s="46" t="s">
+      <c r="E48" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="F48" s="46" t="s">
+      <c r="F48" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="G48" s="46" t="s">
+      <c r="G48" s="23" t="s">
         <v>250</v>
       </c>
-      <c r="H48" s="47">
+      <c r="H48" s="24">
         <v>19</v>
       </c>
-      <c r="I48" s="45" t="s">
+      <c r="I48" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J48" s="46" t="s">
+      <c r="J48" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="K48" s="45" t="s">
+      <c r="K48" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L48" s="45" t="s">
+      <c r="L48" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M48" s="45"/>
-      <c r="N48" s="45" t="s">
+      <c r="M48" s="22"/>
+      <c r="N48" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="O48" s="46"/>
-      <c r="P48" s="46" t="s">
+      <c r="O48" s="23"/>
+      <c r="P48" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q48" s="46">
+      <c r="Q48" s="23">
         <v>6</v>
       </c>
-      <c r="R48" s="46" t="s">
+      <c r="R48" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="S48" s="46" t="s">
+      <c r="S48" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="T48" s="46" t="s">
+      <c r="T48" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="U48" s="46" t="s">
+      <c r="U48" s="23" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="50" t="s">
+    <row r="49" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="53" t="s">
+      <c r="B49" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="C49" s="53" t="s">
+      <c r="C49" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D49" s="53" t="s">
+      <c r="D49" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="E49" s="53" t="s">
+      <c r="E49" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="F49" s="53" t="s">
+      <c r="F49" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="G49" s="53" t="s">
+      <c r="G49" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="H49" s="54">
+      <c r="H49" s="31">
         <v>20</v>
       </c>
-      <c r="I49" s="50" t="s">
+      <c r="I49" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J49" s="53" t="s">
+      <c r="J49" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="K49" s="50" t="s">
+      <c r="K49" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="L49" s="50" t="s">
+      <c r="L49" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M49" s="50"/>
-      <c r="N49" s="51" t="s">
+      <c r="M49" s="27"/>
+      <c r="N49" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="O49" s="53"/>
-      <c r="P49" s="52" t="s">
+      <c r="O49" s="30"/>
+      <c r="P49" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="Q49" s="53">
+      <c r="Q49" s="30">
         <v>6</v>
       </c>
-      <c r="R49" s="53" t="s">
+      <c r="R49" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="S49" s="53" t="s">
+      <c r="S49" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="T49" s="53" t="s">
+      <c r="T49" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="U49" s="53" t="s">
+      <c r="U49" s="30" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3920,62 +3920,62 @@
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="51" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="E51" s="13" t="s">
+      <c r="E51" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="F51" s="9"/>
-      <c r="G51" s="16" t="s">
+      <c r="F51" s="23"/>
+      <c r="G51" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="H51" s="20">
+      <c r="H51" s="24">
         <v>22</v>
       </c>
-      <c r="I51" s="5" t="s">
+      <c r="I51" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="J51" s="17" t="s">
+      <c r="J51" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="K51" s="7" t="s">
+      <c r="K51" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L51" s="6" t="s">
+      <c r="L51" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M51" s="8" t="s">
+      <c r="M51" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="N51" s="8"/>
-      <c r="O51" s="9"/>
-      <c r="P51" s="9" t="s">
+      <c r="N51" s="22"/>
+      <c r="O51" s="23"/>
+      <c r="P51" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q51" s="10">
+      <c r="Q51" s="23">
         <v>6</v>
       </c>
-      <c r="R51" s="11" t="s">
+      <c r="R51" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="S51" s="10" t="s">
+      <c r="S51" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="T51" s="12" t="s">
+      <c r="T51" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="U51" s="10" t="s">
+      <c r="U51" s="23" t="s">
         <v>151</v>
       </c>
     </row>
@@ -4049,127 +4049,127 @@
       <c r="T53" s="12"/>
       <c r="U53" s="10"/>
     </row>
-    <row r="54" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="45" t="s">
+    <row r="54" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B54" s="46" t="s">
+      <c r="B54" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C54" s="46" t="s">
+      <c r="C54" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D54" s="46" t="s">
+      <c r="D54" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="E54" s="46" t="s">
+      <c r="E54" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="F54" s="46" t="s">
+      <c r="F54" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="G54" s="46" t="s">
+      <c r="G54" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="H54" s="47">
+      <c r="H54" s="24">
         <v>23</v>
       </c>
-      <c r="I54" s="45" t="s">
+      <c r="I54" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J54" s="46" t="s">
+      <c r="J54" s="23" t="s">
         <v>302</v>
       </c>
-      <c r="K54" s="45" t="s">
+      <c r="K54" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L54" s="45" t="s">
+      <c r="L54" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M54" s="45"/>
-      <c r="N54" s="45" t="s">
+      <c r="M54" s="22"/>
+      <c r="N54" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="O54" s="46"/>
-      <c r="P54" s="46" t="s">
+      <c r="O54" s="23"/>
+      <c r="P54" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q54" s="46">
+      <c r="Q54" s="23">
         <v>6</v>
       </c>
-      <c r="R54" s="46" t="s">
+      <c r="R54" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="S54" s="46" t="s">
+      <c r="S54" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="T54" s="46" t="s">
+      <c r="T54" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="U54" s="46" t="s">
+      <c r="U54" s="23" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="45" t="s">
+    <row r="55" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="46" t="s">
+      <c r="B55" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C55" s="46" t="s">
+      <c r="C55" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D55" s="46" t="s">
+      <c r="D55" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="E55" s="46" t="s">
+      <c r="E55" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="F55" s="46" t="s">
+      <c r="F55" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="G55" s="46" t="s">
+      <c r="G55" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="H55" s="47">
+      <c r="H55" s="24">
         <v>24</v>
       </c>
-      <c r="I55" s="45" t="s">
+      <c r="I55" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J55" s="46" t="s">
+      <c r="J55" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="K55" s="45" t="s">
+      <c r="K55" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L55" s="45" t="s">
+      <c r="L55" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M55" s="45"/>
-      <c r="N55" s="45" t="s">
+      <c r="M55" s="22"/>
+      <c r="N55" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="O55" s="49" t="s">
+      <c r="O55" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="P55" s="46" t="s">
+      <c r="P55" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="Q55" s="46">
+      <c r="Q55" s="23">
         <v>6</v>
       </c>
-      <c r="R55" s="46" t="s">
+      <c r="R55" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="S55" s="46" t="s">
+      <c r="S55" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="T55" s="46" t="s">
+      <c r="T55" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="U55" s="46" t="s">
+      <c r="U55" s="23" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4348,64 +4348,64 @@
       <c r="T60" s="12"/>
       <c r="U60" s="10"/>
     </row>
-    <row r="61" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="45" t="s">
+    <row r="61" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B61" s="46" t="s">
+      <c r="B61" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C61" s="46" t="s">
+      <c r="C61" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D61" s="46" t="s">
+      <c r="D61" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="E61" s="46" t="s">
+      <c r="E61" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="F61" s="46" t="s">
+      <c r="F61" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="G61" s="46" t="s">
+      <c r="G61" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="H61" s="47">
+      <c r="H61" s="24">
         <v>25</v>
       </c>
-      <c r="I61" s="45" t="s">
+      <c r="I61" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J61" s="46" t="s">
+      <c r="J61" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="K61" s="45" t="s">
+      <c r="K61" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L61" s="45" t="s">
+      <c r="L61" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M61" s="45"/>
-      <c r="N61" s="45" t="s">
+      <c r="M61" s="22"/>
+      <c r="N61" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="O61" s="46"/>
-      <c r="P61" s="46" t="s">
+      <c r="O61" s="23"/>
+      <c r="P61" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q61" s="46">
+      <c r="Q61" s="23">
         <v>6</v>
       </c>
-      <c r="R61" s="46" t="s">
+      <c r="R61" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="S61" s="46" t="s">
+      <c r="S61" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="T61" s="46" t="s">
+      <c r="T61" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="U61" s="46" t="s">
+      <c r="U61" s="23" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4444,125 +4444,125 @@
       <c r="T62" s="12"/>
       <c r="U62" s="10"/>
     </row>
-    <row r="63" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="45" t="s">
+    <row r="63" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B63" s="46" t="s">
+      <c r="B63" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C63" s="46" t="s">
+      <c r="C63" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D63" s="46" t="s">
+      <c r="D63" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="E63" s="46" t="s">
+      <c r="E63" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="F63" s="46" t="s">
+      <c r="F63" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="G63" s="46" t="s">
+      <c r="G63" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="H63" s="47">
+      <c r="H63" s="24">
         <v>26</v>
       </c>
-      <c r="I63" s="45" t="s">
+      <c r="I63" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J63" s="46" t="s">
+      <c r="J63" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="K63" s="45" t="s">
+      <c r="K63" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L63" s="45" t="s">
+      <c r="L63" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M63" s="45"/>
-      <c r="N63" s="45" t="s">
+      <c r="M63" s="22"/>
+      <c r="N63" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="O63" s="46"/>
-      <c r="P63" s="46" t="s">
+      <c r="O63" s="23"/>
+      <c r="P63" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q63" s="46">
+      <c r="Q63" s="23">
         <v>6</v>
       </c>
-      <c r="R63" s="46" t="s">
+      <c r="R63" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="S63" s="46" t="s">
+      <c r="S63" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="T63" s="46" t="s">
+      <c r="T63" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="U63" s="46" t="s">
+      <c r="U63" s="23" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="50" t="s">
+    <row r="64" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B64" s="53" t="s">
+      <c r="B64" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="C64" s="53" t="s">
+      <c r="C64" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D64" s="53" t="s">
+      <c r="D64" s="30" t="s">
         <v>278</v>
       </c>
-      <c r="E64" s="53" t="s">
+      <c r="E64" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="F64" s="53" t="s">
+      <c r="F64" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="G64" s="53" t="s">
+      <c r="G64" s="30" t="s">
         <v>275</v>
       </c>
-      <c r="H64" s="54">
+      <c r="H64" s="31">
         <v>27</v>
       </c>
-      <c r="I64" s="50" t="s">
+      <c r="I64" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J64" s="53" t="s">
+      <c r="J64" s="30" t="s">
         <v>276</v>
       </c>
-      <c r="K64" s="50" t="s">
+      <c r="K64" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="L64" s="50" t="s">
+      <c r="L64" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M64" s="50"/>
-      <c r="N64" s="51" t="s">
+      <c r="M64" s="27"/>
+      <c r="N64" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="O64" s="53"/>
-      <c r="P64" s="52" t="s">
+      <c r="O64" s="30"/>
+      <c r="P64" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="Q64" s="53">
+      <c r="Q64" s="30">
         <v>6</v>
       </c>
-      <c r="R64" s="53" t="s">
+      <c r="R64" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="S64" s="53" t="s">
+      <c r="S64" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="T64" s="53" t="s">
+      <c r="T64" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="U64" s="53" t="s">
+      <c r="U64" s="30" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4789,64 +4789,64 @@
       <c r="T69" s="12"/>
       <c r="U69" s="10"/>
     </row>
-    <row r="70" spans="1:21" s="55" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="50" t="s">
+    <row r="70" spans="1:21" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B70" s="53" t="s">
+      <c r="B70" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="C70" s="53" t="s">
+      <c r="C70" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D70" s="53" t="s">
+      <c r="D70" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="E70" s="53" t="s">
+      <c r="E70" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="F70" s="53" t="s">
+      <c r="F70" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="G70" s="53" t="s">
+      <c r="G70" s="30" t="s">
         <v>286</v>
       </c>
-      <c r="H70" s="54">
+      <c r="H70" s="31">
         <v>30</v>
       </c>
-      <c r="I70" s="50" t="s">
+      <c r="I70" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J70" s="53" t="s">
+      <c r="J70" s="30" t="s">
         <v>287</v>
       </c>
-      <c r="K70" s="50" t="s">
+      <c r="K70" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="L70" s="50" t="s">
+      <c r="L70" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M70" s="50"/>
-      <c r="N70" s="50" t="s">
+      <c r="M70" s="27"/>
+      <c r="N70" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="O70" s="53"/>
-      <c r="P70" s="53" t="s">
+      <c r="O70" s="30"/>
+      <c r="P70" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q70" s="53">
+      <c r="Q70" s="30">
         <v>6</v>
       </c>
-      <c r="R70" s="53" t="s">
+      <c r="R70" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="S70" s="53" t="s">
+      <c r="S70" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="T70" s="53" t="s">
+      <c r="T70" s="30" t="s">
         <v>295</v>
       </c>
-      <c r="U70" s="53" t="s">
+      <c r="U70" s="30" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4909,60 +4909,60 @@
         <v>297</v>
       </c>
     </row>
-    <row r="72" spans="1:21" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="45" t="s">
+    <row r="72" spans="1:21" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B72" s="46" t="s">
+      <c r="B72" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C72" s="46" t="s">
+      <c r="C72" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D72" s="46" t="s">
+      <c r="D72" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="E72" s="46"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="46" t="s">
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="H72" s="47">
+      <c r="H72" s="24">
         <v>32</v>
       </c>
-      <c r="I72" s="45" t="s">
+      <c r="I72" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J72" s="46" t="s">
+      <c r="J72" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="K72" s="45" t="s">
+      <c r="K72" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="L72" s="45" t="s">
+      <c r="L72" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M72" s="45"/>
-      <c r="N72" s="45" t="s">
+      <c r="M72" s="22"/>
+      <c r="N72" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="O72" s="46"/>
-      <c r="P72" s="46" t="s">
+      <c r="O72" s="23"/>
+      <c r="P72" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="Q72" s="46">
+      <c r="Q72" s="23">
         <v>6</v>
       </c>
-      <c r="R72" s="46" t="s">
+      <c r="R72" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="S72" s="46" t="s">
+      <c r="S72" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="T72" s="46" t="s">
+      <c r="T72" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="U72" s="46" t="s">
+      <c r="U72" s="23" t="s">
         <v>140</v>
       </c>
     </row>
@@ -5543,12 +5543,6 @@
     <row r="289" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5563,6 +5557,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O55" r:id="rId1"/>

</xml_diff>